<commit_message>
Fixed safety factor being incorrect
</commit_message>
<xml_diff>
--- a/RearVD.xlsx
+++ b/RearVD.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,32 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\timot\Documents\Projects\Git\Wishbone-Forces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A302DC-4856-41A9-95E8-6279B3AB43C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B3132171-D359-46D9-9975-DC64464DE61F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="348" yWindow="1728" windowWidth="23040" windowHeight="12204"/>
   </bookViews>
   <sheets>
     <sheet name="OutputForces" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
   <si>
     <t>Scenario</t>
   </si>
@@ -108,6 +95,9 @@
   </si>
   <si>
     <t>Corner Inner Brake Bump</t>
+  </si>
+  <si>
+    <t>Accelerate and below</t>
   </si>
   <si>
     <t>Max compression</t>
@@ -191,7 +181,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -696,6 +686,9 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -704,9 +697,6 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1061,30 +1051,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.44140625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
@@ -1663,37 +1637,37 @@
         <v>25</v>
       </c>
       <c r="C14">
-        <v>-1500</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>-1500</v>
+        <v>0</v>
       </c>
       <c r="E14">
         <v>750</v>
       </c>
       <c r="F14">
-        <v>-200</v>
+        <v>0</v>
       </c>
       <c r="G14">
-        <v>-1351.10819353888</v>
+        <v>-59.135406112003601</v>
       </c>
       <c r="H14">
-        <v>-1158.02062627137</v>
+        <v>200.25132491294599</v>
       </c>
       <c r="I14">
-        <v>-1790.7769821632801</v>
+        <v>-182.591149437768</v>
       </c>
       <c r="J14">
-        <v>-5419.7410021055703</v>
+        <v>-743.212781566697</v>
       </c>
       <c r="K14">
-        <v>936.473576411267</v>
-      </c>
-      <c r="L14">
-        <v>-637.61337677257302</v>
+        <v>1068.1737277131399</v>
+      </c>
+      <c r="L14" s="1">
+        <v>9.1612915170680105E-12</v>
       </c>
       <c r="M14">
-        <v>96.946732237505202</v>
+        <v>244.85769893052901</v>
       </c>
       <c r="N14">
         <v>595.44235304784195</v>
@@ -1704,363 +1678,891 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15">
+        <v>750</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>750</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>664.70908521999104</v>
+      </c>
+      <c r="H15">
+        <v>-171.997965310795</v>
+      </c>
+      <c r="I15">
+        <v>-2533.04747224116</v>
+      </c>
+      <c r="J15">
+        <v>636.07296783575396</v>
+      </c>
+      <c r="K15">
+        <v>1068.0647777997899</v>
+      </c>
+      <c r="L15">
+        <v>198.95261820202899</v>
+      </c>
+      <c r="M15">
+        <v>793.31437571462402</v>
+      </c>
+      <c r="N15">
+        <v>3092.79491279372</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>750</v>
+      </c>
+      <c r="F16">
+        <v>-200</v>
+      </c>
+      <c r="G16">
+        <v>111.76858773235701</v>
+      </c>
+      <c r="H16">
+        <v>130.72552415847699</v>
+      </c>
+      <c r="I16">
+        <v>-16.682174690643201</v>
+      </c>
+      <c r="J16">
+        <v>-636.38667119867</v>
+      </c>
+      <c r="K16">
+        <v>1068.30499605913</v>
+      </c>
+      <c r="L16">
+        <v>-239.70814036853201</v>
+      </c>
+      <c r="M16">
+        <v>96.946732237505202</v>
+      </c>
+      <c r="N16">
+        <v>622.24019855165795</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17">
+        <v>1500</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>750</v>
+      </c>
+      <c r="F17">
+        <v>-200</v>
+      </c>
+      <c r="G17">
+        <v>1559.4575703963401</v>
+      </c>
+      <c r="H17">
+        <v>-613.77305628900501</v>
+      </c>
+      <c r="I17">
+        <v>-4717.5948202974296</v>
+      </c>
+      <c r="J17">
+        <v>2122.1848276062301</v>
+      </c>
+      <c r="K17">
+        <v>1068.08709623243</v>
+      </c>
+      <c r="L17">
+        <v>158.197096035507</v>
+      </c>
+      <c r="M17">
+        <v>2032.4308784842201</v>
+      </c>
+      <c r="N17">
+        <v>6619.1209788217302</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>1500</v>
+      </c>
+      <c r="E18">
+        <v>750</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>-439.70980188227799</v>
+      </c>
+      <c r="H18">
+        <v>1488.9974753428</v>
+      </c>
+      <c r="I18">
+        <v>1425.5946832877401</v>
+      </c>
+      <c r="J18">
+        <v>-4602.3698967318996</v>
+      </c>
+      <c r="K18">
+        <v>1199.8738790150101</v>
+      </c>
+      <c r="L18" s="1">
+        <v>9.0908400598998995E-11</v>
+      </c>
+      <c r="M18">
+        <v>1820.67457323588</v>
+      </c>
+      <c r="N18">
+        <v>5864.3057079115097</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19">
+        <v>1060</v>
+      </c>
+      <c r="D19">
+        <v>1060</v>
+      </c>
+      <c r="E19">
+        <v>750</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>694.95890195955496</v>
+      </c>
+      <c r="H19">
+        <v>584.85294103382103</v>
+      </c>
+      <c r="I19">
+        <v>-2368.1180972072002</v>
+      </c>
+      <c r="J19">
+        <v>-1520.95995046131</v>
+      </c>
+      <c r="K19">
+        <v>1161.08785208893</v>
+      </c>
+      <c r="L19">
+        <v>281.18636705892197</v>
+      </c>
+      <c r="M19">
+        <v>513.39898419568306</v>
+      </c>
+      <c r="N19">
+        <v>1336.4547696890399</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>1500</v>
+      </c>
+      <c r="E20">
+        <v>750</v>
+      </c>
+      <c r="F20">
+        <v>-200</v>
+      </c>
+      <c r="G20">
+        <v>-268.80580803791599</v>
+      </c>
+      <c r="H20">
+        <v>1419.47167458833</v>
+      </c>
+      <c r="I20">
+        <v>1591.5036580348701</v>
+      </c>
+      <c r="J20">
+        <v>-4495.5437863638699</v>
+      </c>
+      <c r="K20">
+        <v>1200.0051473609999</v>
+      </c>
+      <c r="L20">
+        <v>-239.70814036845101</v>
+      </c>
+      <c r="M20">
+        <v>1616.85560928224</v>
+      </c>
+      <c r="N20">
+        <v>5910.1436970086697</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21">
+        <v>1060</v>
+      </c>
+      <c r="D21">
+        <v>1060</v>
+      </c>
+      <c r="E21">
+        <v>750</v>
+      </c>
+      <c r="F21">
+        <v>-200</v>
+      </c>
+      <c r="G21">
+        <v>865.86289580391599</v>
+      </c>
+      <c r="H21">
+        <v>515.32714027935299</v>
+      </c>
+      <c r="I21">
+        <v>-2202.2091224600699</v>
+      </c>
+      <c r="J21">
+        <v>-1414.13384009328</v>
+      </c>
+      <c r="K21">
+        <v>1161.2191204349199</v>
+      </c>
+      <c r="L21">
+        <v>41.478226690380197</v>
+      </c>
+      <c r="M21">
+        <v>631.60494796823195</v>
+      </c>
+      <c r="N21">
+        <v>1242.9232003530999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>-1500</v>
+      </c>
+      <c r="E22">
+        <v>750</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>321.438989658271</v>
+      </c>
+      <c r="H22">
+        <v>-1088.4948255168999</v>
+      </c>
+      <c r="I22">
+        <v>-1790.7769821632801</v>
+      </c>
+      <c r="J22">
+        <v>3115.9443335985002</v>
+      </c>
+      <c r="K22">
+        <v>936.473576411267</v>
+      </c>
+      <c r="L22" s="1">
+        <v>-7.2585817564863003E-11</v>
+      </c>
+      <c r="M22">
+        <v>1330.95917537482</v>
+      </c>
+      <c r="N22">
+        <v>4735.04864403802</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23">
+        <v>1060</v>
+      </c>
+      <c r="D23">
+        <v>-1060</v>
+      </c>
+      <c r="E23">
+        <v>750</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>1232.8373813148701</v>
+      </c>
+      <c r="H23">
+        <v>-1236.5749515737</v>
+      </c>
+      <c r="I23">
+        <v>-4641.0207407926</v>
+      </c>
+      <c r="J23">
+        <v>3933.3154389721699</v>
+      </c>
+      <c r="K23">
+        <v>974.95163824894996</v>
+      </c>
+      <c r="L23">
+        <v>281.18636705880601</v>
+      </c>
+      <c r="M23">
+        <v>2270.42873909625</v>
+      </c>
+      <c r="N23">
+        <v>8252.5289400097699</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>-1500</v>
+      </c>
+      <c r="E24">
+        <v>750</v>
+      </c>
+      <c r="F24">
+        <v>-200</v>
+      </c>
+      <c r="G24">
+        <v>492.34298350263202</v>
+      </c>
+      <c r="H24">
+        <v>-1158.02062627137</v>
+      </c>
+      <c r="I24">
+        <v>-1624.86800741616</v>
+      </c>
+      <c r="J24">
+        <v>3222.7704439665299</v>
+      </c>
+      <c r="K24">
+        <v>936.60484475726003</v>
+      </c>
+      <c r="L24">
+        <v>-239.70814036861401</v>
+      </c>
+      <c r="M24">
+        <v>1539.79638887957</v>
+      </c>
+      <c r="N24">
+        <v>4684.68047103956</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25">
+        <v>1060</v>
+      </c>
+      <c r="D25">
+        <v>-1060</v>
+      </c>
+      <c r="E25">
+        <v>750</v>
+      </c>
+      <c r="F25">
+        <v>-200</v>
+      </c>
+      <c r="G25">
+        <v>1403.7413751592301</v>
+      </c>
+      <c r="H25">
+        <v>-1306.1007523281701</v>
+      </c>
+      <c r="I25">
+        <v>-4475.1117660454702</v>
+      </c>
+      <c r="J25">
+        <v>4040.1415493402001</v>
+      </c>
+      <c r="K25">
+        <v>975.08290659494196</v>
+      </c>
+      <c r="L25">
+        <v>41.478226690264698</v>
+      </c>
+      <c r="M25">
+        <v>2491.7802375000801</v>
+      </c>
+      <c r="N25">
+        <v>8194.2845539849095</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
         <v>26</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
+      <c r="C26">
+        <v>-1500</v>
+      </c>
+      <c r="D26">
+        <v>-1500</v>
+      </c>
+      <c r="E26">
+        <v>750</v>
+      </c>
+      <c r="F26">
+        <v>-200</v>
+      </c>
+      <c r="G26">
+        <v>-1351.10819353888</v>
+      </c>
+      <c r="H26">
+        <v>-1306.1007523281701</v>
+      </c>
+      <c r="I26">
+        <v>-4717.5948202974296</v>
+      </c>
+      <c r="J26">
+        <v>-5419.7410021055703</v>
+      </c>
+      <c r="K26">
+        <v>936.473576411267</v>
+      </c>
+      <c r="L26">
+        <v>-637.61337677257302</v>
+      </c>
+      <c r="M26">
+        <v>96.946732237505202</v>
+      </c>
+      <c r="N26">
+        <v>595.44235304784195</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27">
         <v>1500</v>
       </c>
-      <c r="E15">
-        <v>750</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>492.34298350263202</v>
-      </c>
-      <c r="H15">
+      <c r="D27">
+        <v>1500</v>
+      </c>
+      <c r="E27">
+        <v>750</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>1559.4575703963401</v>
+      </c>
+      <c r="H27">
         <v>1637.0776013995901</v>
       </c>
-      <c r="I15">
+      <c r="I27">
         <v>4684.2304709161399</v>
       </c>
-      <c r="J15">
-        <v>3222.7704439665299</v>
-      </c>
-      <c r="K15">
+      <c r="J27">
+        <v>4040.1415493402001</v>
+      </c>
+      <c r="K27">
         <v>1200.0051473609999</v>
       </c>
-      <c r="L15" s="1">
-        <v>9.0908400598998995E-11</v>
-      </c>
-      <c r="M15">
+      <c r="L27">
+        <v>281.18636705892197</v>
+      </c>
+      <c r="M27">
         <v>2749.7001208574202</v>
       </c>
-      <c r="N15">
+      <c r="N27">
         <v>9388.9929324024397</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="G16" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B17" s="2" t="s">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G28" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="3">
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B29" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="4">
         <v>210000000000</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B30" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="4">
         <v>240000000</v>
       </c>
-      <c r="G18" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10" t="s">
+      <c r="G30" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J18" s="10"/>
-      <c r="K18" s="2" t="s">
+      <c r="H30" s="2"/>
+      <c r="I30" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L18" s="2" t="s">
+      <c r="J30" s="2"/>
+      <c r="K30" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="N18" s="2" t="s">
+      <c r="L30" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="F19" s="2" t="s">
+      <c r="N30" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G19" s="4">
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F31" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G31" s="5">
         <v>275</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H31" s="5">
         <v>278</v>
       </c>
-      <c r="I19" s="4">
+      <c r="I31" s="5">
         <v>391</v>
       </c>
-      <c r="J19" s="4">
+      <c r="J31" s="5">
         <v>436</v>
       </c>
-      <c r="K19" s="4">
+      <c r="K31" s="5">
         <v>584</v>
       </c>
-      <c r="L19" s="4">
+      <c r="L31" s="5">
         <v>329</v>
       </c>
-      <c r="N19" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B20" s="2" t="s">
+      <c r="N31" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="4">
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B32" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="5">
         <v>2</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G20" s="4">
-        <v>5</v>
-      </c>
-      <c r="H20" s="4">
-        <v>5</v>
-      </c>
-      <c r="I20" s="4">
-        <v>5</v>
-      </c>
-      <c r="J20" s="4">
-        <v>5</v>
-      </c>
-      <c r="K20" s="4">
-        <v>5</v>
-      </c>
-      <c r="L20" s="4">
-        <v>5</v>
-      </c>
-      <c r="N20" s="5" t="s">
+      <c r="F32" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B21" s="2" t="s">
+      <c r="G32" s="5">
+        <v>0</v>
+      </c>
+      <c r="H32" s="5">
+        <v>0</v>
+      </c>
+      <c r="I32" s="5">
+        <v>0</v>
+      </c>
+      <c r="J32" s="5">
+        <v>0</v>
+      </c>
+      <c r="K32" s="5">
+        <v>0</v>
+      </c>
+      <c r="L32" s="5">
+        <v>0</v>
+      </c>
+      <c r="N32" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="4">
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B33" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="5">
         <v>2</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F21" s="2" t="s">
+      <c r="E33" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="6">
-        <f>-G14*(G19/1000)^2/(PI()^2*$C$17/$C$20)</f>
-        <v>9.8597628864194258E-11</v>
-      </c>
-      <c r="H21" s="6">
-        <f t="shared" ref="H21:L21" si="0">-H14*(H19/1000)^2/(PI()^2*$C$17/$C$20)</f>
-        <v>8.6360836905796107E-11</v>
-      </c>
-      <c r="I21" s="6">
+      <c r="F33" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G33" s="7">
+        <f>-G26*(G31/1000)^2/(PI()^2*$C$29)</f>
+        <v>4.9298814432097129E-11</v>
+      </c>
+      <c r="H33" s="7">
+        <f t="shared" ref="H33:L33" si="0">-H26*(H31/1000)^2/(PI()^2*$C$29)</f>
+        <v>4.8702048778498245E-11</v>
+      </c>
+      <c r="I33" s="7">
         <f t="shared" si="0"/>
-        <v>2.6418367293027706E-10</v>
-      </c>
-      <c r="J21" s="6">
+        <v>3.4798066410186542E-10</v>
+      </c>
+      <c r="J33" s="7">
         <f t="shared" si="0"/>
-        <v>9.9417415103819187E-10</v>
-      </c>
-      <c r="K21" s="6">
+        <v>4.9708707551909594E-10</v>
+      </c>
+      <c r="K33" s="7">
         <f t="shared" si="0"/>
-        <v>-3.0819967582322838E-10</v>
-      </c>
-      <c r="L21" s="6">
+        <v>-1.5409983791161419E-10</v>
+      </c>
+      <c r="L33" s="7">
         <f t="shared" si="0"/>
-        <v>6.6597844211777214E-11</v>
-      </c>
-      <c r="N21" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B22" s="2" t="s">
+        <v>3.3298922105888607E-11</v>
+      </c>
+      <c r="N33" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="4">
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B34" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="5">
         <v>2</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G22" s="8">
-        <f t="shared" ref="G22:J22" si="1">IF(G21&gt;0,(2*G21*$C$20/PI()+(G20/1000)^4)^0.25*1000,"Tension only")</f>
-        <v>5.2341146249890516</v>
-      </c>
-      <c r="H22" s="8">
+      <c r="F34" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G34" s="9">
+        <f>IF(G33&gt;0,(2*G33*$C$32/PI()+(G32/1000)^4)^0.25*1000,"Tension only")</f>
+        <v>2.8147293941316387</v>
+      </c>
+      <c r="H34" s="9">
+        <f t="shared" ref="H34:L34" si="1">IF(H33&gt;0,(2*H33*$C$32/PI()+(H32/1000)^4)^0.25*1000,"Tension only")</f>
+        <v>2.8061723267508043</v>
+      </c>
+      <c r="I34" s="9">
         <f t="shared" si="1"/>
-        <v>5.2067369261529892</v>
-      </c>
-      <c r="I22" s="8">
+        <v>4.5879249793660195</v>
+      </c>
+      <c r="J34" s="9">
         <f t="shared" si="1"/>
-        <v>5.5682989005072878</v>
-      </c>
-      <c r="J22" s="8">
+        <v>5.0157472939534564</v>
+      </c>
+      <c r="K34" s="9" t="str">
         <f t="shared" si="1"/>
-        <v>6.5942081639107819</v>
-      </c>
-      <c r="K22" s="8" t="str">
-        <f>IF(K21&gt;0,(2*K21*$C$20/PI()+(K20/1000)^4)^0.25*1000,"Tension only")</f>
         <v>Tension only</v>
       </c>
-      <c r="L22" s="8">
-        <f>IF(L21&gt;0,(2*L21*$C$20/PI()+(L20/1000)^4)^0.25*1000,"Tension only")</f>
-        <v>5.1615868025998717</v>
-      </c>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="E23" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F23" s="2" t="s">
+      <c r="L34" s="9">
+        <f t="shared" si="1"/>
+        <v>2.5517320799740491</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="E35" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G23" s="6">
-        <f t="shared" ref="G23:L23" si="2">G15/$C$18</f>
-        <v>2.0514290979276336E-6</v>
-      </c>
-      <c r="H23" s="6">
-        <f t="shared" si="2"/>
+      <c r="F35" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G35" s="7">
+        <f>G27/$C$30</f>
+        <v>6.4977398766514173E-6</v>
+      </c>
+      <c r="H35" s="7">
+        <f t="shared" ref="H35:L35" si="2">H27/$C$30</f>
         <v>6.8211566724982921E-6</v>
       </c>
-      <c r="I23" s="6">
+      <c r="I35" s="7">
         <f t="shared" si="2"/>
         <v>1.9517626962150582E-5</v>
       </c>
-      <c r="J23" s="6">
+      <c r="J35" s="7">
         <f t="shared" si="2"/>
-        <v>1.3428210183193874E-5</v>
-      </c>
-      <c r="K23" s="6">
+        <v>1.6833923122250833E-5</v>
+      </c>
+      <c r="K35" s="7">
         <f t="shared" si="2"/>
         <v>5.0000214473374994E-6</v>
       </c>
-      <c r="L23" s="6">
+      <c r="L35" s="7">
         <f t="shared" si="2"/>
-        <v>3.7878500249582914E-19</v>
-      </c>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="F24" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G24" s="8">
-        <f>(4*G23*$C$21/PI()+(G20/1000)^2)^0.5*1000</f>
-        <v>5.4976286980300602</v>
-      </c>
-      <c r="H24" s="8">
-        <f t="shared" ref="H24:L24" si="3">(4*H23*$C$21/PI()+(H20/1000)^2)^0.5*1000</f>
-        <v>6.5092190647202743</v>
-      </c>
-      <c r="I24" s="8">
+        <v>1.1716098627455081E-6</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="F36" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G36" s="9">
+        <f>(4*G35*$C$33/PI()+(G32/1000)^2)^0.5*1000</f>
+        <v>4.0677215643048052</v>
+      </c>
+      <c r="H36" s="9">
+        <f t="shared" ref="H36:L36" si="3">(4*H35*$C$33/PI()+(H32/1000)^2)^0.5*1000</f>
+        <v>4.1677251387918908</v>
+      </c>
+      <c r="I36" s="9">
         <f t="shared" si="3"/>
-        <v>8.6429872691794873</v>
-      </c>
-      <c r="J24" s="8">
+        <v>7.049909852983844</v>
+      </c>
+      <c r="J36" s="9">
         <f t="shared" si="3"/>
-        <v>7.6938063687953369</v>
-      </c>
-      <c r="K24" s="8">
+        <v>6.5473073262649555</v>
+      </c>
+      <c r="K36" s="9">
         <f t="shared" si="3"/>
-        <v>6.1426745040371538</v>
-      </c>
-      <c r="L24" s="8">
+        <v>3.5682558852397475</v>
+      </c>
+      <c r="L36" s="9">
         <f t="shared" si="3"/>
-        <v>5.0000000000000968</v>
-      </c>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="E25" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F25" s="2" t="s">
+        <v>1.7272753157787657</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="E37" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G25" s="9">
-        <f t="shared" ref="G25:L25" si="4">MAX(G24,G22)</f>
-        <v>5.4976286980300602</v>
-      </c>
-      <c r="H25" s="9">
+      <c r="F37" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G37" s="10">
+        <f t="shared" ref="G37:L37" si="4">MAX(G36,G34)</f>
+        <v>4.0677215643048052</v>
+      </c>
+      <c r="H37" s="10">
         <f t="shared" si="4"/>
-        <v>6.5092190647202743</v>
-      </c>
-      <c r="I25" s="9">
+        <v>4.1677251387918908</v>
+      </c>
+      <c r="I37" s="10">
         <f t="shared" si="4"/>
-        <v>8.6429872691794873</v>
-      </c>
-      <c r="J25" s="9">
+        <v>7.049909852983844</v>
+      </c>
+      <c r="J37" s="10">
         <f t="shared" si="4"/>
-        <v>7.6938063687953369</v>
-      </c>
-      <c r="K25" s="9">
+        <v>6.5473073262649555</v>
+      </c>
+      <c r="K37" s="10">
         <f t="shared" si="4"/>
-        <v>6.1426745040371538</v>
-      </c>
-      <c r="L25" s="9">
+        <v>3.5682558852397475</v>
+      </c>
+      <c r="L37" s="10">
         <f t="shared" si="4"/>
-        <v>5.1615868025998717</v>
-      </c>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="G27" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="G28" s="7">
-        <f>MAX(ABS(G14),ABS(G15))*$C$22</f>
-        <v>2702.2163870777599</v>
-      </c>
-      <c r="H28" s="7">
-        <f t="shared" ref="H28:N28" si="5">MAX(ABS(H14),ABS(H15))*$C$22</f>
+        <v>2.5517320799740491</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="G39" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="G40" s="8">
+        <f>MAX(ABS(G26),ABS(G27))*$C$34</f>
+        <v>3118.9151407926802</v>
+      </c>
+      <c r="H40" s="8">
+        <f t="shared" ref="H40:J40" si="5">MAX(ABS(H26),ABS(H27))*$C$34</f>
         <v>3274.1552027991802</v>
       </c>
-      <c r="I28" s="7">
+      <c r="I40" s="8">
         <f t="shared" si="5"/>
-        <v>9368.4609418322798</v>
-      </c>
-      <c r="J28" s="7">
+        <v>9435.1896405948592</v>
+      </c>
+      <c r="J40" s="8">
         <f t="shared" si="5"/>
         <v>10839.482004211141</v>
       </c>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="7">
-        <f t="shared" si="5"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="8">
+        <f>MAX(ABS(M26),ABS(M27))*$C$34</f>
         <v>5499.4002417148404</v>
       </c>
-      <c r="N28" s="7">
-        <f t="shared" si="5"/>
+      <c r="N40" s="8">
+        <f>MAX(ABS(N26),ABS(N27))*$C$34</f>
         <v>18777.985864804879</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="G16:N16"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="G27:N27"/>
+    <mergeCell ref="G28:N28"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="G39:N39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>